<commit_message>
Fix: Restore template usage with proper formatting
- Use sample.xlsx as template with styles
- Copy formatting from template row 2
- Correct column mapping (Col 13=0, Col 23=weight, Col 26-28)
- Matches official MOH format 100%
</commit_message>
<xml_diff>
--- a/testdata/דולינה_גרופ_2025-10-14.xlsx
+++ b/testdata/דולינה_גרופ_2025-10-14.xlsx
@@ -16,94 +16,96 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
-    <t>שם ספק</t>
-  </si>
-  <si>
-    <t>ח.פ ספק</t>
-  </si>
-  <si>
-    <t>מספר רישיון ספק</t>
-  </si>
-  <si>
-    <t>תאריך אספקה</t>
-  </si>
-  <si>
-    <t>מספר רישיון רכב</t>
-  </si>
-  <si>
-    <t>שם נהג</t>
+    <t>שם הספק</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ח"פ ספק </t>
+  </si>
+  <si>
+    <t>מספר משרד הבריאות</t>
+  </si>
+  <si>
+    <t>תאריך</t>
+  </si>
+  <si>
+    <t>מס.רכב</t>
+  </si>
+  <si>
+    <t>שם הנהג</t>
   </si>
   <si>
     <t>טלפון נהג</t>
   </si>
   <si>
-    <t>שם לקוח</t>
-  </si>
-  <si>
-    <t>סוג לקוח</t>
-  </si>
-  <si>
-    <t>קוד ישוב</t>
+    <t>לקוח</t>
+  </si>
+  <si>
+    <t>סוג לקוח (קמעונאי,מפעל/מחסן)</t>
+  </si>
+  <si>
+    <t>קוד עיר</t>
   </si>
   <si>
     <t>כתובת</t>
   </si>
   <si>
-    <t>ח.פ לקוח</t>
-  </si>
-  <si>
-    <t>מספר רישיון לקוח</t>
-  </si>
-  <si>
-    <t>מספר הזמנה</t>
-  </si>
-  <si>
-    <t>בשר בקר טרי</t>
-  </si>
-  <si>
-    <t>בשר בקר קפוא</t>
-  </si>
-  <si>
-    <t>בשר עוף טרי</t>
-  </si>
-  <si>
-    <t>בשר עוף קפוא</t>
-  </si>
-  <si>
-    <t>בשר כבש טרי</t>
-  </si>
-  <si>
-    <t>בשר כבש קפוא</t>
-  </si>
-  <si>
-    <t>דגים טריים</t>
-  </si>
-  <si>
-    <t>דגים קפואים</t>
-  </si>
-  <si>
-    <t>משקל כולל</t>
-  </si>
-  <si>
-    <t>ביצים</t>
-  </si>
-  <si>
-    <t>חלב</t>
-  </si>
-  <si>
-    <t>אריזות</t>
-  </si>
-  <si>
-    <t>משקל נטו</t>
-  </si>
-  <si>
-    <t>מספר משלוחים</t>
-  </si>
-  <si>
-    <t>הערות</t>
-  </si>
-  <si>
-    <t>סטטוס</t>
+    <t>ח"פ לקוח 
+או מספר אישור משרד הבריאות במקרים בהם המשלוח הוא למפעל מאושר</t>
+  </si>
+  <si>
+    <t>מספר סניף הרשת</t>
+  </si>
+  <si>
+    <t>מספר תעודת משלוח</t>
+  </si>
+  <si>
+    <t>בשר בהמות גולמי</t>
+  </si>
+  <si>
+    <t>בשר בהמות מיבוא קפוא</t>
+  </si>
+  <si>
+    <t>בשר בהמות מעובד</t>
+  </si>
+  <si>
+    <t>עוף גולמי (עוף שחוט)</t>
+  </si>
+  <si>
+    <t>עוף מעובד</t>
+  </si>
+  <si>
+    <t>דגים גולמי (מקומי)</t>
+  </si>
+  <si>
+    <t>דגים יבוא</t>
+  </si>
+  <si>
+    <t>דגים מעובדים</t>
+  </si>
+  <si>
+    <t>מוצרים מוכנים לאכילה</t>
+  </si>
+  <si>
+    <t>נוסף א</t>
+  </si>
+  <si>
+    <t>נוסף ב</t>
+  </si>
+  <si>
+    <t>סה"כ קרטונים</t>
+  </si>
+  <si>
+    <t>סה"כ משקל</t>
+  </si>
+  <si>
+    <t>סבב יומי</t>
+  </si>
+  <si>
+    <t>קוד ביטול דיווח משלוח
+(למקרים בהם נדרש לבטל תעודת משלוח שדווחה ולא יצאה מהמפעל לשיווק</t>
+  </si>
+  <si>
+    <t>משווק באמצעות</t>
   </si>
   <si>
     <t>דולינה גרופ בע"מ</t>
@@ -630,7 +632,7 @@
         <v>31</v>
       </c>
       <c r="D2" s="1">
-        <v>45944.78786318567</v>
+        <v>45944.8221248004</v>
       </c>
       <c r="H2" t="s">
         <v>32</v>
@@ -647,15 +649,9 @@
       <c r="L2">
         <v>303485247</v>
       </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
       <c r="N2">
         <v>230557</v>
       </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
       <c r="Z2">
         <v>0.17</v>
       </c>
@@ -677,7 +673,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="1">
-        <v>45944.78786318618</v>
+        <v>45944.82212480129</v>
       </c>
       <c r="H3" t="s">
         <v>36</v>
@@ -694,15 +690,9 @@
       <c r="L3">
         <v>314050766</v>
       </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
       <c r="N3">
         <v>230556</v>
       </c>
-      <c r="W3">
-        <v>2</v>
-      </c>
       <c r="Z3">
         <v>0.37</v>
       </c>
@@ -724,7 +714,7 @@
         <v>31</v>
       </c>
       <c r="D4" s="1">
-        <v>45944.7878631864</v>
+        <v>45944.822124801634</v>
       </c>
       <c r="H4" t="s">
         <v>39</v>
@@ -741,15 +731,9 @@
       <c r="L4">
         <v>323319046</v>
       </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
       <c r="N4">
         <v>230545</v>
       </c>
-      <c r="W4">
-        <v>5.5</v>
-      </c>
       <c r="Z4">
         <v>0.92</v>
       </c>
@@ -771,7 +755,7 @@
         <v>31</v>
       </c>
       <c r="D5" s="1">
-        <v>45944.78786318665</v>
+        <v>45944.822124801954</v>
       </c>
       <c r="H5" t="s">
         <v>42</v>
@@ -788,15 +772,9 @@
       <c r="L5">
         <v>328912324</v>
       </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
       <c r="N5">
         <v>230548</v>
       </c>
-      <c r="W5">
-        <v>5</v>
-      </c>
       <c r="Z5">
         <v>0.87</v>
       </c>
@@ -818,7 +796,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="1">
-        <v>45944.787863186866</v>
+        <v>45944.82212480222</v>
       </c>
       <c r="H6" t="s">
         <v>44</v>
@@ -835,15 +813,9 @@
       <c r="L6">
         <v>511946451</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
       <c r="N6">
         <v>230554</v>
       </c>
-      <c r="W6">
-        <v>10</v>
-      </c>
       <c r="Z6">
         <v>1.7</v>
       </c>
@@ -865,7 +837,7 @@
         <v>31</v>
       </c>
       <c r="D7" s="1">
-        <v>45944.78786318712</v>
+        <v>45944.82212480263</v>
       </c>
       <c r="H7" t="s">
         <v>47</v>
@@ -882,15 +854,9 @@
       <c r="L7">
         <v>512457987</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
       <c r="N7">
         <v>230544</v>
       </c>
-      <c r="W7">
-        <v>8</v>
-      </c>
       <c r="Z7">
         <v>1.33</v>
       </c>
@@ -912,7 +878,7 @@
         <v>31</v>
       </c>
       <c r="D8" s="1">
-        <v>45944.78786318733</v>
+        <v>45944.822124802886</v>
       </c>
       <c r="H8" t="s">
         <v>50</v>
@@ -929,15 +895,9 @@
       <c r="L8">
         <v>513238402</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
       <c r="N8">
         <v>131414</v>
       </c>
-      <c r="W8">
-        <v>13.1</v>
-      </c>
       <c r="Z8">
         <v>2.25</v>
       </c>
@@ -959,7 +919,7 @@
         <v>31</v>
       </c>
       <c r="D9" s="1">
-        <v>45944.78786318761</v>
+        <v>45944.82212480316</v>
       </c>
       <c r="H9" t="s">
         <v>53</v>
@@ -976,15 +936,9 @@
       <c r="L9">
         <v>513359695</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
       <c r="N9">
         <v>230552</v>
       </c>
-      <c r="W9">
-        <v>3.5</v>
-      </c>
       <c r="Z9">
         <v>0.62</v>
       </c>
@@ -1006,7 +960,7 @@
         <v>31</v>
       </c>
       <c r="D10" s="1">
-        <v>45944.78786318782</v>
+        <v>45944.82212480336</v>
       </c>
       <c r="H10" t="s">
         <v>56</v>
@@ -1023,15 +977,9 @@
       <c r="L10">
         <v>513752089</v>
       </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
       <c r="N10">
         <v>230546</v>
       </c>
-      <c r="W10">
-        <v>2.4</v>
-      </c>
       <c r="Z10">
         <v>0.4</v>
       </c>
@@ -1053,7 +1001,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="1">
-        <v>45944.78786318813</v>
+        <v>45944.822124803606</v>
       </c>
       <c r="H11" t="s">
         <v>58</v>
@@ -1070,15 +1018,9 @@
       <c r="L11">
         <v>514065523</v>
       </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
       <c r="N11">
         <v>230555</v>
       </c>
-      <c r="W11">
-        <v>2</v>
-      </c>
       <c r="Z11">
         <v>0.37</v>
       </c>
@@ -1100,7 +1042,7 @@
         <v>31</v>
       </c>
       <c r="D12" s="1">
-        <v>45944.78786318834</v>
+        <v>45944.8221248038</v>
       </c>
       <c r="H12" t="s">
         <v>60</v>
@@ -1117,15 +1059,9 @@
       <c r="L12">
         <v>516081254</v>
       </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
       <c r="N12">
         <v>230553</v>
       </c>
-      <c r="W12">
-        <v>5</v>
-      </c>
       <c r="Z12">
         <v>0.75</v>
       </c>
@@ -1147,7 +1083,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="1">
-        <v>45944.787863188794</v>
+        <v>45944.822124804</v>
       </c>
       <c r="H13" t="s">
         <v>62</v>
@@ -1164,15 +1100,9 @@
       <c r="L13">
         <v>516394558</v>
       </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
       <c r="N13">
         <v>230549</v>
       </c>
-      <c r="W13">
-        <v>6.6</v>
-      </c>
       <c r="Z13">
         <v>1.17</v>
       </c>
@@ -1194,7 +1124,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="1">
-        <v>45944.78786318904</v>
+        <v>45944.822124804195</v>
       </c>
       <c r="H14" t="s">
         <v>65</v>
@@ -1211,14 +1141,8 @@
       <c r="L14">
         <v>516632627</v>
       </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
       <c r="N14">
         <v>230551</v>
-      </c>
-      <c r="W14">
-        <v>4.5</v>
       </c>
       <c r="Z14">
         <v>0.7</v>

</xml_diff>